<commit_message>
Commiting changes - 12 Dec
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -9,6 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="Movie" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t xml:space="preserve">FilmName</t>
   </si>
@@ -34,7 +37,7 @@
     <t xml:space="preserve">Heroin</t>
   </si>
   <si>
-    <t xml:space="preserve">Age</t>
+    <t xml:space="preserve">ReleaseYear</t>
   </si>
   <si>
     <t xml:space="preserve">RRR</t>
@@ -65,6 +68,21 @@
   </si>
   <si>
     <t xml:space="preserve">Rashmika</t>
+  </si>
+  <si>
+    <t>Bimbisara</t>
+  </si>
+  <si>
+    <t>Kalyan Ram</t>
+  </si>
+  <si>
+    <t>Mallidi Vassishta</t>
+  </si>
+  <si>
+    <t>Samyuktha Menon</t>
+  </si>
+  <si>
+    <t>2022</t>
   </si>
 </sst>
 </file>
@@ -162,19 +180,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1048332" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="10.61" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="1025" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -205,7 +223,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>20</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -222,7 +240,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>30</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,7 +257,24 @@
         <v>14</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>40</v>
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -251,4 +286,82 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>